<commit_message>
submit gnn for all datasets
</commit_message>
<xml_diff>
--- a/baselines/results_old/extracted_data_with_variance.xlsx
+++ b/baselines/results_old/extracted_data_with_variance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenshao/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C7E765-C136-0141-9121-876EE8CBF294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA12276E-F57A-4C46-B3AA-B93000CDC420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="760" windowWidth="24560" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4680" yWindow="-18560" windowWidth="29040" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="115">
   <si>
     <t>Metric</t>
   </si>
@@ -332,13 +332,46 @@
   </si>
   <si>
     <t>49.84 ± 15.56</t>
+  </si>
+  <si>
+    <t>Internal:</t>
+  </si>
+  <si>
+    <t>copy from NCNC paper with split 70/10/20</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>copy from HearT paper table 1</t>
+  </si>
+  <si>
+    <t>my experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low confidence without double check </t>
+  </si>
+  <si>
+    <t xml:space="preserve">copy from NCNC has big gap with our previous work, certainly needs to be double checked </t>
+  </si>
+  <si>
+    <t>LPFormer</t>
+  </si>
+  <si>
+    <t>MPLP</t>
+  </si>
+  <si>
+    <t>Computer</t>
+  </si>
+  <si>
+    <t>Photo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,16 +396,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
+      <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -402,14 +472,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,24 +789,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A18" sqref="A17:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="4" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -745,357 +820,486 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="H7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="I7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="J7" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>80</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="H8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I9" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J9" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J10" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J11" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J12" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D13" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J13" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I14" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J14" s="4" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>